<commit_message>
highlight: Add latest highlight reports
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/proj_time_plan.xlsx
+++ b/docs/proj_time_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\uni\vmicro16\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8407D0-771A-407A-9451-B63091EA9AFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1A7C5E-37F2-4189-83EB-758B36976FEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{F166F07A-0375-4A16-B899-B830BBC88168}"/>
   </bookViews>
@@ -2077,11 +2077,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.49459</cdr:x>
+      <cdr:x>0.55391</cdr:x>
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.50465</cdr:x>
+      <cdr:x>0.56397</cdr:x>
       <cdr:y>1</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -2097,8 +2097,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5007787" y="0"/>
-          <a:ext cx="101858" cy="7341534"/>
+          <a:off x="5608396" y="0"/>
+          <a:ext cx="101859" cy="7341534"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>

</xml_diff>

<commit_message>
interim: updated gantt chart
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/proj_time_plan.xlsx
+++ b/docs/proj_time_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\uni\vmicro16\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8E44FB-EEE8-4D21-A575-6682629B2674}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711C095C-5043-4BA0-ACF0-22BB8BC0052F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{F166F07A-0375-4A16-B899-B830BBC88168}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>(CORE) Research</t>
+  </si>
+  <si>
+    <t>Intense Coursework/Exam month</t>
   </si>
 </sst>
 </file>
@@ -265,9 +268,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$2:$B$24</c:f>
+              <c:f>Sheet1!$A$2:$B$25</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>(CORE) Research</c:v>
@@ -306,36 +309,39 @@
                     <c:v>(CORE) Cache memory design &amp; impl</c:v>
                   </c:pt>
                   <c:pt idx="12">
+                    <c:v>Intense Coursework/Exam month</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>(CORE) Multi-core communication interface</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="14">
                     <c:v>(CORE) Shared-memory controller</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="15">
                     <c:v>(CORE) Scalable multi-core interface (10s of cores)</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="16">
                     <c:v>(CORE) Multi-core example program (reduction)</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="17">
                     <c:v>(EXT) SPI-FPGA interface for OTG programming</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="18">
                     <c:v>(EXT) FPGA-PC interfacing</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="19">
                     <c:v>(EXT) FPGA-PC debugging (instruction breakpoints)</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="20">
                     <c:v>(EXT) Compiler backend for vmicro16</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="21">
                     <c:v>(EXT) Compiler support for multi-core codegen</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="22">
                     <c:v>(CORE) Wishbone peripherals for demo</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="23">
                     <c:v>Final Report</c:v>
                   </c:pt>
                 </c:lvl>
@@ -377,36 +383,39 @@
                     <c:v>3.4</c:v>
                   </c:pt>
                   <c:pt idx="12">
+                    <c:v>X</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>4.1</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="14">
                     <c:v>4.2</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="15">
                     <c:v>4.3</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="16">
                     <c:v>4.4</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="17">
                     <c:v>5.1</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="18">
                     <c:v>5.2</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="19">
                     <c:v>5.3</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="20">
                     <c:v>6.1</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="21">
                     <c:v>6.2</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="22">
                     <c:v>7.1</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="23">
                     <c:v>8</c:v>
                   </c:pt>
                 </c:lvl>
@@ -415,10 +424,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$24</c:f>
+              <c:f>Sheet1!$C$2:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>43500</c:v>
                 </c:pt>
@@ -452,14 +461,26 @@
                 <c:pt idx="10">
                   <c:v>43570</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>43577</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="12">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43621</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43621</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43647</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43656</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>43678</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>43535</c:v>
+                <c:pt idx="23">
+                  <c:v>43621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -496,9 +517,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$2:$B$24</c:f>
+              <c:f>Sheet1!$A$2:$B$25</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>(CORE) Research</c:v>
@@ -537,36 +558,39 @@
                     <c:v>(CORE) Cache memory design &amp; impl</c:v>
                   </c:pt>
                   <c:pt idx="12">
+                    <c:v>Intense Coursework/Exam month</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>(CORE) Multi-core communication interface</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="14">
                     <c:v>(CORE) Shared-memory controller</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="15">
                     <c:v>(CORE) Scalable multi-core interface (10s of cores)</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="16">
                     <c:v>(CORE) Multi-core example program (reduction)</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="17">
                     <c:v>(EXT) SPI-FPGA interface for OTG programming</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="18">
                     <c:v>(EXT) FPGA-PC interfacing</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="19">
                     <c:v>(EXT) FPGA-PC debugging (instruction breakpoints)</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="20">
                     <c:v>(EXT) Compiler backend for vmicro16</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="21">
                     <c:v>(EXT) Compiler support for multi-core codegen</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="22">
                     <c:v>(CORE) Wishbone peripherals for demo</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="23">
                     <c:v>Final Report</c:v>
                   </c:pt>
                 </c:lvl>
@@ -608,36 +632,39 @@
                     <c:v>3.4</c:v>
                   </c:pt>
                   <c:pt idx="12">
+                    <c:v>X</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>4.1</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="14">
                     <c:v>4.2</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="15">
                     <c:v>4.3</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="16">
                     <c:v>4.4</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="17">
                     <c:v>5.1</c:v>
                   </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="18">
                     <c:v>5.2</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="19">
                     <c:v>5.3</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="20">
                     <c:v>6.1</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="21">
                     <c:v>6.2</c:v>
                   </c:pt>
-                  <c:pt idx="21">
+                  <c:pt idx="22">
                     <c:v>7.1</c:v>
                   </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="23">
                     <c:v>8</c:v>
                   </c:pt>
                 </c:lvl>
@@ -646,10 +673,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$24</c:f>
+              <c:f>Sheet1!$D$2:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
@@ -683,29 +710,41 @@
                 <c:pt idx="10">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>28</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28</c:v>
+                </c:pt>
                 <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="22">
-                  <c:v>150</c:v>
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1523,7 +1562,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1556,12 +1595,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0</cdr:x>
-      <cdr:y>0.39689</cdr:y>
+      <cdr:x>0.00081</cdr:x>
+      <cdr:y>0.37895</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.96982</cdr:x>
-      <cdr:y>0.70885</cdr:y>
+      <cdr:x>0.97063</cdr:x>
+      <cdr:y>0.52941</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1576,8 +1615,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="2913765"/>
-          <a:ext cx="9819501" cy="2290248"/>
+          <a:off x="8283" y="3028372"/>
+          <a:ext cx="9874123" cy="1202386"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1619,7 +1658,7 @@
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0.00188</cdr:x>
-      <cdr:y>0.70762</cdr:y>
+      <cdr:y>0.56879</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.9717</cdr:x>
@@ -1638,8 +1677,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="19035" y="5195049"/>
-          <a:ext cx="9819501" cy="860612"/>
+          <a:off x="19141" y="4545497"/>
+          <a:ext cx="9874123" cy="2046271"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1771,12 +1810,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0</cdr:x>
-      <cdr:y>0.24239</cdr:y>
+      <cdr:x>0.00081</cdr:x>
+      <cdr:y>0.22995</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.96982</cdr:x>
-      <cdr:y>0.35595</cdr:y>
+      <cdr:x>0.97063</cdr:x>
+      <cdr:y>0.34389</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1791,8 +1830,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="1779495"/>
-          <a:ext cx="9819501" cy="833718"/>
+          <a:off x="8282" y="1837663"/>
+          <a:ext cx="9874123" cy="910508"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1929,7 +1968,7 @@
     </cdr:from>
     <cdr:to>
       <cdr:x>0.96982</cdr:x>
-      <cdr:y>0.23872</cdr:y>
+      <cdr:y>0.23092</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1944,8 +1983,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="611048"/>
-          <a:ext cx="9819501" cy="1141553"/>
+          <a:off x="0" y="665131"/>
+          <a:ext cx="9874123" cy="1180236"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2077,11 +2116,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.55391</cdr:x>
+      <cdr:x>0.59133</cdr:x>
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.56397</cdr:x>
+      <cdr:x>0.60139</cdr:x>
       <cdr:y>1</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -2097,8 +2136,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5608396" y="0"/>
-          <a:ext cx="101859" cy="7341534"/>
+          <a:off x="6020578" y="0"/>
+          <a:ext cx="102425" cy="7991475"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2289,12 +2328,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0</cdr:x>
-      <cdr:y>0.35656</cdr:y>
+      <cdr:x>0.00081</cdr:x>
+      <cdr:y>0.34234</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.96982</cdr:x>
-      <cdr:y>0.39747</cdr:y>
+      <cdr:x>0.97063</cdr:x>
+      <cdr:y>0.3812</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2309,8 +2348,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="2617707"/>
-          <a:ext cx="9819501" cy="300306"/>
+          <a:off x="8283" y="2735770"/>
+          <a:ext cx="9874123" cy="310574"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2623,6 +2662,159 @@
         </a:prstGeom>
         <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:srgbClr val="00B050">
+            <a:alpha val="15000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:noFill/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.52872</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.96982</cdr:x>
+      <cdr:y>0.56758</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13C351A7-E910-4FAB-9717-095A55956CE8}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="4225235"/>
+          <a:ext cx="9874123" cy="310574"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:srgbClr val="FF0000">
             <a:alpha val="15000"/>
           </a:srgbClr>
         </a:solidFill>
@@ -3046,10 +3238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81979E81-6286-4617-9260-EEEC38151FA0}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3232,83 +3424,97 @@
       <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4">
-        <v>43577</v>
-      </c>
-      <c r="D13" s="3">
-        <v>28</v>
-      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="1"/>
+      <c r="A14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="7">
+        <v>43586</v>
+      </c>
+      <c r="D14" s="6">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="C15" s="2">
+        <v>43621</v>
+      </c>
+      <c r="D15" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C16" s="2">
+        <v>43621</v>
+      </c>
+      <c r="D16" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="C17" s="2">
+        <v>43647</v>
+      </c>
+      <c r="D17" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2">
+        <v>43656</v>
+      </c>
+      <c r="D18" s="1">
         <v>7</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="3">
-        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>5.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="3">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="3">
@@ -3316,55 +3522,67 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>6.1</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="1">
-        <v>7</v>
+      <c r="A21" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="3">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>6.2</v>
+        <v>6.1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="1">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>7.1</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="4">
-        <v>43678</v>
-      </c>
-      <c r="D23" s="3">
-        <v>7</v>
+      <c r="A23" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="1">
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="4">
+        <v>43678</v>
+      </c>
+      <c r="D24" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>8</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="2">
-        <v>43535</v>
-      </c>
-      <c r="D24" s="1">
-        <v>150</v>
+      <c r="C25" s="2">
+        <v>43621</v>
+      </c>
+      <c r="D25" s="1">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
interim: start of intro
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/docs/proj_time_plan.xlsx
+++ b/docs/proj_time_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\uni\vmicro16\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711C095C-5043-4BA0-ACF0-22BB8BC0052F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997C1AFC-36A3-4CB9-870A-F611AFE64907}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{F166F07A-0375-4A16-B899-B830BBC88168}"/>
   </bookViews>
@@ -1964,7 +1964,7 @@
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0</cdr:x>
-      <cdr:y>0.08323</cdr:y>
+      <cdr:y>0.07856</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.96982</cdr:x>
@@ -1983,8 +1983,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="665131"/>
-          <a:ext cx="9874123" cy="1180236"/>
+          <a:off x="0" y="627823"/>
+          <a:ext cx="9874123" cy="1217544"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -3241,7 +3241,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>